<commit_message>
wireless tls and results reset
</commit_message>
<xml_diff>
--- a/results/averages.xlsx
+++ b/results/averages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\DNSSecExt\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199A2AEC-F905-4DC5-8319-67C283692D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224E9AAF-A3FA-4AE7-90A1-15B8ABAF7A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="17">
   <si>
     <t>DNS Server</t>
   </si>
@@ -69,17 +69,14 @@
     <t>average RTT time of query</t>
   </si>
   <si>
-    <t>Second Run
+    <t>~9501 hits</t>
+  </si>
+  <si>
+    <t>Cached Run
 -&gt;</t>
   </si>
   <si>
-    <t>~9489 hits</t>
-  </si>
-  <si>
-    <t>~9501 hits</t>
-  </si>
-  <si>
-    <t>~9483 hits</t>
+    <t>~ 9488 hits</t>
   </si>
 </sst>
 </file>
@@ -299,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -338,6 +335,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -365,10 +365,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,7 +651,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +679,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>3</v>
@@ -705,19 +701,19 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28"/>
       <c r="H2" s="20"/>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="28"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D3" s="12" t="s">
@@ -749,76 +745,34 @@
       <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="29" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="8"/>
-      <c r="D4" s="13">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="E4" s="8">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0.09</v>
-      </c>
-      <c r="G4" s="7">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="13">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="J4" s="8">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="K4" s="8">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="L4" s="7">
-        <v>8.6999999999999994E-2</v>
-      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="7"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="7"/>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="D5" s="12">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="E5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F5">
-        <v>0.89</v>
-      </c>
-      <c r="G5" s="6">
-        <v>7.8E-2</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="12">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="J5">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="K5">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="L5" s="6">
-        <v>7.0000000000000007E-2</v>
-      </c>
+      <c r="B5" s="30"/>
+      <c r="D5" s="12"/>
+      <c r="G5" s="6"/>
+      <c r="I5" s="12"/>
+      <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="30"/>
+      <c r="B6" s="31"/>
       <c r="C6" s="3"/>
       <c r="D6" s="11"/>
       <c r="E6" s="3"/>
@@ -845,19 +799,19 @@
     </row>
     <row r="9" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="25"/>
       <c r="H9" s="20"/>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="25"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
@@ -890,47 +844,45 @@
       <c r="A11" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="13">
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8">
-        <v>0.104</v>
-      </c>
-      <c r="G11" s="7">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="H11" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="13">
-        <v>0.106</v>
-      </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="L11" s="7">
-        <v>0.109</v>
-      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="8">
+        <v>0.111</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="7"/>
+      <c r="H11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="13"/>
+      <c r="J11" s="8">
+        <v>0.108</v>
+      </c>
+      <c r="K11" s="8"/>
+      <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="30"/>
+      <c r="B12" s="31"/>
       <c r="C12" s="3"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="14"/>
-      <c r="H12" s="32"/>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
       <c r="I12" s="11"/>
-      <c r="J12" s="3"/>
+      <c r="J12" s="3">
+        <v>7.3999999999999996E-2</v>
+      </c>
       <c r="K12" s="3"/>
       <c r="L12" s="14"/>
     </row>

</xml_diff>

<commit_message>
self hosted update - possible need for redo
</commit_message>
<xml_diff>
--- a/results/averages.xlsx
+++ b/results/averages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\DNSSecExt\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72DC128-D24F-4852-8E25-C3EB25F16F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7022D847-70EA-4D31-B836-80A28A68FCA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
   <si>
     <t>DNS Server</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>WiFi Connection</t>
-  </si>
-  <si>
-    <t>[ms]</t>
   </si>
   <si>
     <t>average RTT time of query</t>
@@ -83,6 +80,12 @@
   </si>
   <si>
     <t>~9489 hits</t>
+  </si>
+  <si>
+    <t>10000 hits</t>
+  </si>
+  <si>
+    <t>[s]</t>
   </si>
 </sst>
 </file>
@@ -657,7 +660,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N12" sqref="N12"/>
+      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,7 +688,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>3</v>
@@ -708,14 +711,14 @@
         <v>2</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="27"/>
       <c r="F2" s="27"/>
       <c r="G2" s="28"/>
       <c r="H2" s="20"/>
       <c r="I2" s="26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J2" s="27"/>
       <c r="K2" s="27"/>
@@ -723,28 +726,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D3" s="12" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="K3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -768,7 +771,7 @@
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I4" s="13">
         <v>9.4E-2</v>
@@ -801,7 +804,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I5" s="12">
         <v>7.0999999999999994E-2</v>
@@ -822,14 +825,33 @@
       </c>
       <c r="B6" s="31"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="14"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="14"/>
+      <c r="D6" s="11">
+        <v>1.14E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.1299999999999999E-3</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1.41E-3</v>
+      </c>
+      <c r="G6" s="14">
+        <v>1.33E-3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="11">
+        <v>1.16E-3</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1.42E-3</v>
+      </c>
+      <c r="L6" s="14">
+        <v>1.31E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
@@ -848,14 +870,14 @@
     <row r="9" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="D9" s="23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
       <c r="G9" s="25"/>
       <c r="H9" s="20"/>
       <c r="I9" s="23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J9" s="24"/>
       <c r="K9" s="24"/>
@@ -864,28 +886,28 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="D10" s="12" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="J10" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="K10" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -909,7 +931,7 @@
         <v>0.105</v>
       </c>
       <c r="H11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I11" s="13">
         <v>0.10299999999999999</v>
@@ -943,7 +965,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="H12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I12" s="11">
         <v>6.7000000000000004E-2</v>

</xml_diff>